<commit_message>
1.3 Updated files for parameters Hypertuning
</commit_message>
<xml_diff>
--- a/datafile/tabella risultati.xlsx
+++ b/datafile/tabella risultati.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Desktop\SentAnalys\datafile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401514FC-3045-41B4-BD36-FDEBD73BF5AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE89CDA4-6138-4D17-9EFA-69F83283E354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -111,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="90">
   <si>
     <t>Model</t>
   </si>
@@ -186,6 +186,201 @@
   </si>
   <si>
     <t>Count Vectorization, train-set: 80%</t>
+  </si>
+  <si>
+    <t>Count Vectorization, train-set: 80%, After Parameter Hypertuning</t>
+  </si>
+  <si>
+    <t>New Parameters: C=8,35989 (default=1); penalty= 'l2' (default), solver='sag' (default= 'lbfgs').</t>
+  </si>
+  <si>
+    <t>1st try: scikit-optimize</t>
+  </si>
+  <si>
+    <t>Anche aumentando "max_iter" a 500 il modello non converge</t>
+  </si>
+  <si>
+    <t>2nd try: test manuale</t>
+  </si>
+  <si>
+    <t>C=6.5</t>
+  </si>
+  <si>
+    <t>Tuning aumentando max_df da 0.80 a 0.99 nel CountVectorizer</t>
+  </si>
+  <si>
+    <t>{'max_df': 0.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'accuracy': 0.9128</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'F1': 0.9127189745836984</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'TPR': 0.9214</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'TNR': 0.9044}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>{'max_df': 0.81</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'accuracy': 0.9124</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'F1': 0.912275398695676</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'TPR': 0.9206</t>
+  </si>
+  <si>
+    <t>{'max_df': 0.8200000000000001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'accuracy': 0.9121</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'F1': 0.9119771723041501</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'TPR': 0.9202</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'TNR': 0.9042}</t>
+  </si>
+  <si>
+    <t>{'max_df': 0.8300000000000001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'accuracy': 0.9129</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'F1': 0.9128245371891773</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'TPR': 0.9212</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'TNR': 0.9048}</t>
+  </si>
+  <si>
+    <t>{'max_df': 0.8400000000000001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'F1': 0.9126754313886607</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'TPR': 0.921</t>
+  </si>
+  <si>
+    <t>{'max_df': 0.8500000000000001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'accuracy': 0.9123</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'F1': 0.9121771882707591</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'TPR': 0.9204</t>
+  </si>
+  <si>
+    <t>{'max_df': 0.8600000000000001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'accuracy': 0.9127</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'F1': 0.9125807483701308</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'TNR': 0.905}</t>
+  </si>
+  <si>
+    <t>{'max_df': 0.8700000000000001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'accuracy': 0.9126</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'F1': 0.9124754150457509</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'TPR': 0.9208</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'TNR': 0.9046}</t>
+  </si>
+  <si>
+    <t>{'max_df': 0.8800000000000001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'accuracy': 0.9122</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'F1': 0.9121226485419864</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'TNR': 0.904}</t>
+  </si>
+  <si>
+    <t>{'max_df': 0.8900000000000001</t>
+  </si>
+  <si>
+    <t>{'max_df': 0.9000000000000001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'F1': 0.9120753823384311</t>
+  </si>
+  <si>
+    <t>{'max_df': 0.9100000000000001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'F1': 0.9123226654975888</t>
+  </si>
+  <si>
+    <t>{'max_df': 0.9200000000000002</t>
+  </si>
+  <si>
+    <t>{'max_df': 0.9300000000000002</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'F1': 0.9120244710009867</t>
+  </si>
+  <si>
+    <t>{'max_df': 0.9400000000000002</t>
+  </si>
+  <si>
+    <t>{'max_df': 0.9500000000000002</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'F1': 0.9121807180049328</t>
+  </si>
+  <si>
+    <t>{'max_df': 0.9600000000000002</t>
+  </si>
+  <si>
+    <t>{'max_df': 0.9700000000000002</t>
+  </si>
+  <si>
+    <t>{'max_df': 0.9800000000000002</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'accuracy': 0.9125</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'F1': 0.9123772042303688</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'TNR': 0.9046}]</t>
+  </si>
+  <si>
+    <t>Ridotto il range di test: C=[5,6,6.5,7,8] aumentando max_iter=700</t>
   </si>
 </sst>
 </file>
@@ -195,7 +390,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,13 +446,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -292,7 +500,7 @@
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -346,6 +554,9 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -358,7 +569,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Migliaia" xfId="1" builtinId="3"/>
@@ -644,7 +864,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -683,7 +903,7 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="22" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -714,7 +934,7 @@
       <c r="K2" s="4"/>
     </row>
     <row r="3" spans="1:11" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="19"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
@@ -743,7 +963,7 @@
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="19"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
@@ -772,7 +992,7 @@
       <c r="K4" s="4"/>
     </row>
     <row r="5" spans="1:11" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="22" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -803,7 +1023,7 @@
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" ht="52" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="19"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
@@ -832,7 +1052,7 @@
       <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:11" ht="43" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="19"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
@@ -902,7 +1122,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="31.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="22" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -919,7 +1139,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="19"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
@@ -934,7 +1154,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="19"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
@@ -949,7 +1169,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="37.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="22" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -966,7 +1186,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="47.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="19"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
@@ -981,7 +1201,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="19"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
@@ -1009,8 +1229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EF9A79F-94F3-40D5-B9E4-4F108E221FD5}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:L9"/>
+    <sheetView zoomScale="81" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1136,77 +1356,77 @@
       <c r="K4" s="4"/>
     </row>
     <row r="5" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
       <c r="M5" s="9"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="8"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
       <c r="M6" s="9"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="8"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
       <c r="M7" s="9"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
       <c r="M8" s="9"/>
     </row>
     <row r="9" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
       <c r="M9" s="9"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
@@ -1237,7 +1457,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView zoomScale="102" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="I2" sqref="I2:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1279,7 +1499,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="22" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1314,7 +1534,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="19"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
@@ -1347,7 +1567,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="19"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
@@ -1380,7 +1600,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="22" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1415,7 +1635,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="19"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
@@ -1448,7 +1668,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="19"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
@@ -1533,7 +1753,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="22" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1577,7 +1797,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="19"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
@@ -1619,7 +1839,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="19"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
@@ -1661,7 +1881,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="22" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1705,7 +1925,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="19"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
@@ -1747,7 +1967,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="19"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
@@ -1826,7 +2046,7 @@
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1870,7 +2090,7 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="22" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1905,7 +2125,7 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="19"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
@@ -1938,7 +2158,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="19"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
@@ -1969,17 +2189,17 @@
       <c r="K4" s="12">
         <v>0.62509999999999999</v>
       </c>
-      <c r="N4" s="19" t="s">
+      <c r="N4" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="19"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
     </row>
     <row r="5" spans="1:19" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="19"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
@@ -2010,15 +2230,15 @@
       <c r="K5" s="10">
         <v>0.88190000000000002</v>
       </c>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="19"/>
-      <c r="S5" s="19"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="22"/>
     </row>
     <row r="6" spans="1:19" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="19"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
@@ -2051,7 +2271,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="19"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="3" t="s">
         <v>22</v>
       </c>
@@ -2084,7 +2304,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="21"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
@@ -2117,7 +2337,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="25" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="16" t="s">
@@ -2152,7 +2372,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" ht="32.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="19"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
@@ -2185,7 +2405,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" ht="32.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="19"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="3" t="s">
         <v>11</v>
       </c>
@@ -2218,7 +2438,7 @@
       </c>
     </row>
     <row r="12" spans="1:19" ht="31.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="19"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="3" t="s">
         <v>19</v>
       </c>
@@ -2251,7 +2471,7 @@
       </c>
     </row>
     <row r="13" spans="1:19" ht="33.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="19"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="3" t="s">
         <v>20</v>
       </c>
@@ -2284,7 +2504,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="19"/>
+      <c r="A14" s="22"/>
       <c r="B14" s="3" t="s">
         <v>22</v>
       </c>
@@ -2317,7 +2537,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="19"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="3" t="s">
         <v>23</v>
       </c>
@@ -2407,7 +2627,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="43" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="22" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -2451,7 +2671,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="19"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
@@ -2493,7 +2713,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="19"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
@@ -2535,7 +2755,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="22" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -2579,7 +2799,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="19"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
@@ -2621,7 +2841,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="19"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
@@ -2697,21 +2917,24 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D69DA31-7454-4880-ADD3-932A3DF016AA}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="13.7265625" customWidth="1"/>
+    <col min="1" max="1" width="13.90625" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" customWidth="1"/>
+    <col min="3" max="3" width="13.90625" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
+    <col min="5" max="5" width="13.36328125" customWidth="1"/>
     <col min="7" max="9" width="12.453125" customWidth="1"/>
     <col min="10" max="10" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
       <c r="B1" s="7" t="s">
         <v>0</v>
@@ -2744,8 +2967,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -2763,44 +2986,457 @@
       <c r="F2">
         <v>392</v>
       </c>
-      <c r="G2" s="23">
+      <c r="G2" s="19">
         <v>0.91080000000000005</v>
       </c>
-      <c r="H2" s="23">
+      <c r="H2" s="19">
         <v>0.92079999999999995</v>
       </c>
-      <c r="I2" s="23">
+      <c r="I2" s="19">
         <v>0.90100000000000002</v>
       </c>
-      <c r="J2" s="23">
+      <c r="J2" s="19">
         <v>0.90110000000000001</v>
       </c>
-      <c r="K2" s="23">
+      <c r="K2" s="19">
         <v>0.91084349305669898</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="19"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="19"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="19"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="19"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="19"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="21"/>
+    <row r="3" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="56" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="20">
+        <v>4558</v>
+      </c>
+      <c r="D4" s="20">
+        <v>484</v>
+      </c>
+      <c r="E4" s="20">
+        <v>4567</v>
+      </c>
+      <c r="F4" s="20">
+        <v>391</v>
+      </c>
+      <c r="G4" s="21">
+        <v>0.91249999999999998</v>
+      </c>
+      <c r="H4" s="21">
+        <v>0.92100000000000004</v>
+      </c>
+      <c r="I4" s="21">
+        <v>0.9042</v>
+      </c>
+      <c r="J4" s="21">
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="K4" s="21">
+        <v>0.91239999999999999</v>
+      </c>
+      <c r="M4" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="R4" s="27"/>
+      <c r="S4" s="27"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>4555</v>
+      </c>
+      <c r="D6">
+        <v>486</v>
+      </c>
+      <c r="E6">
+        <v>4565</v>
+      </c>
+      <c r="F6">
+        <v>394</v>
+      </c>
+      <c r="G6" s="19">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="H6" s="19">
+        <v>0.9204</v>
+      </c>
+      <c r="I6" s="19">
+        <v>0.90380000000000005</v>
+      </c>
+      <c r="J6" s="19">
+        <v>0.90359999999999996</v>
+      </c>
+      <c r="K6" s="19">
+        <v>0.91190000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A8" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A12" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" t="s">
+        <v>88</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:A8"/>
+  <mergeCells count="3">
+    <mergeCell ref="M4:P4"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="A8:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>